<commit_message>
Fix Master Data Validation
</commit_message>
<xml_diff>
--- a/src/main/resources/static/templates/Customer_Import_Template.xlsx
+++ b/src/main/resources/static/templates/Customer_Import_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\S\F\CP\Development\CP_GSM\GSM\src\main\resources\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56CFF7-352E-40F7-B2FD-E11248775598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC3C2EE-60FB-4327-9F46-120BBEA52624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BE228B5D-7B2E-413D-BD1B-3C93BAEBA16D}"/>
   </bookViews>
@@ -36,21 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>CustomerCode</t>
-  </si>
-  <si>
-    <t>CustomerName</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ContactPhone</t>
   </si>
   <si>
     <t>ContactEmail</t>
+  </si>
+  <si>
+    <t>CustomerCode*</t>
+  </si>
+  <si>
+    <t>CustomerName*</t>
+  </si>
+  <si>
+    <t>Address*</t>
+  </si>
+  <si>
+    <t>DeliveryTerm</t>
+  </si>
+  <si>
+    <t>PaymentTerm</t>
+  </si>
+  <si>
+    <t>CurrencyCode*</t>
+  </si>
+  <si>
+    <t>CountryCode*</t>
   </si>
 </sst>
 </file>
@@ -92,10 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,40 +443,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A38314E-120C-45FE-863E-864917086534}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>